<commit_message>
Major Updates 4th April 2016
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qureshi\Documents\SI Labs\SI-Labs-TimeTable\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
   <si>
     <t>Teacher Name</t>
   </si>
@@ -440,6 +445,15 @@
   </si>
   <si>
     <t>HU104B</t>
+  </si>
+  <si>
+    <t>CS666</t>
+  </si>
+  <si>
+    <t>Test Course</t>
+  </si>
+  <si>
+    <t>test111</t>
   </si>
 </sst>
 </file>
@@ -541,6 +555,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -588,7 +605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,7 +640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,6 +1703,20 @@
         <v>120</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D61" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Load Batch File into DB
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qureshi\Documents\SI Labs\SI-Labs-TimeTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samiq\Documents\GitHub\SI-Labs-TimeTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="123">
   <si>
     <t>Teacher Name</t>
   </si>
@@ -330,72 +330,6 @@
     <t>CS6</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test7</t>
-  </si>
-  <si>
-    <t>test8</t>
-  </si>
-  <si>
-    <t>test9</t>
-  </si>
-  <si>
-    <t>test10</t>
-  </si>
-  <si>
-    <t>test11</t>
-  </si>
-  <si>
-    <t>test12</t>
-  </si>
-  <si>
-    <t>test13</t>
-  </si>
-  <si>
-    <t>test14</t>
-  </si>
-  <si>
-    <t>test15</t>
-  </si>
-  <si>
-    <t>test16</t>
-  </si>
-  <si>
-    <t>test17</t>
-  </si>
-  <si>
-    <t>test18</t>
-  </si>
-  <si>
-    <t>test19</t>
-  </si>
-  <si>
-    <t>test20</t>
-  </si>
-  <si>
-    <t>test21</t>
-  </si>
-  <si>
-    <t>test22</t>
-  </si>
-  <si>
     <t>CS102A-L1</t>
   </si>
   <si>
@@ -453,7 +387,7 @@
     <t>Test Course</t>
   </si>
   <si>
-    <t>test111</t>
+    <t>Cno</t>
   </si>
 </sst>
 </file>
@@ -849,872 +783,926 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>72</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>138</v>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>141</v>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>125</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>126</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>71</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>127</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>128</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>72</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>71</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>72</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>129</v>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>71</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>130</v>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>131</v>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>72</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>54</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>74</v>
       </c>
-      <c r="D20" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>132</v>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>133</v>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>74</v>
       </c>
-      <c r="D22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>74</v>
       </c>
-      <c r="D24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>134</v>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>73</v>
       </c>
-      <c r="D27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>135</v>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>74</v>
       </c>
-      <c r="D28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>62</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>73</v>
       </c>
-      <c r="D29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>74</v>
       </c>
-      <c r="D30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>136</v>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" t="s">
         <v>63</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>73</v>
       </c>
-      <c r="D31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>137</v>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>73</v>
       </c>
-      <c r="D33" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>67</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>74</v>
       </c>
-      <c r="D34" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>12</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>19</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>70</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>75</v>
       </c>
-      <c r="D36" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>76</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>75</v>
       </c>
-      <c r="D37" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>77</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>75</v>
       </c>
-      <c r="D38" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>15</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>78</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>75</v>
       </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>16</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>79</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>75</v>
       </c>
-      <c r="D40" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>17</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>75</v>
       </c>
-      <c r="D41" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>18</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>83</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>75</v>
       </c>
-      <c r="D42" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>20</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>84</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>80</v>
       </c>
-      <c r="D43" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>21</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>80</v>
       </c>
-      <c r="D44" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>26</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>80</v>
       </c>
-      <c r="D45" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>22</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>86</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>80</v>
       </c>
-      <c r="D46" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>24</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>88</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>80</v>
       </c>
-      <c r="D47" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>23</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>89</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>80</v>
       </c>
-      <c r="D48" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>25</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>90</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>80</v>
       </c>
-      <c r="D49" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" t="s">
+        <v>96</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" t="s">
-        <v>91</v>
-      </c>
-      <c r="C50" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" t="s">
-        <v>94</v>
-      </c>
-      <c r="C53" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C61" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" t="s">
-        <v>95</v>
-      </c>
-      <c r="C54" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>32</v>
-      </c>
-      <c r="B55" t="s">
-        <v>96</v>
-      </c>
-      <c r="C55" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>33</v>
-      </c>
-      <c r="B56" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B57" t="s">
-        <v>98</v>
-      </c>
-      <c r="C57" t="s">
-        <v>102</v>
-      </c>
-      <c r="D57" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" t="s">
-        <v>102</v>
-      </c>
-      <c r="D58" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>36</v>
-      </c>
-      <c r="B59" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" t="s">
-        <v>102</v>
-      </c>
-      <c r="D59" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>37</v>
-      </c>
-      <c r="B60" t="s">
-        <v>101</v>
-      </c>
-      <c r="C60" t="s">
-        <v>102</v>
-      </c>
-      <c r="D60" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>142</v>
-      </c>
-      <c r="B61" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>75</v>
-      </c>
-      <c r="D61" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DBWriter Functionality: Get Batch Number
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="123">
-  <si>
-    <t>Teacher Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="118">
   <si>
     <t>Nizamuddin</t>
   </si>
@@ -135,15 +132,6 @@
     <t>MT301</t>
   </si>
   <si>
-    <t>Batch</t>
-  </si>
-  <si>
-    <t>Course Title</t>
-  </si>
-  <si>
-    <t>Course Code</t>
-  </si>
-  <si>
     <t>Calculus</t>
   </si>
   <si>
@@ -385,9 +373,6 @@
   </si>
   <si>
     <t>Test Course</t>
-  </si>
-  <si>
-    <t>Cno</t>
   </si>
 </sst>
 </file>
@@ -403,21 +388,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -425,60 +404,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,912 +728,895 @@
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>27</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>31</v>
       </c>
       <c r="C54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D54" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D55" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D56" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>34</v>
       </c>
       <c r="C57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" t="s">
         <v>98</v>
-      </c>
-      <c r="D57" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D58" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D59" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="D60" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Load Schedule (Whew! Lots of Reused Code)
</commit_message>
<xml_diff>
--- a/CSCourseTeachers.xlsx
+++ b/CSCourseTeachers.xlsx
@@ -324,55 +324,55 @@
     <t>Test Course</t>
   </si>
   <si>
-    <t>CS102L-A1</t>
-  </si>
-  <si>
-    <t>CS102L-A2</t>
-  </si>
-  <si>
-    <t>CS102L-B1</t>
-  </si>
-  <si>
-    <t>CS102L-B2</t>
-  </si>
-  <si>
-    <t>CS101L-A1</t>
-  </si>
-  <si>
-    <t>CS101L-A2</t>
-  </si>
-  <si>
-    <t>CS101L-B</t>
-  </si>
-  <si>
-    <t>CS103L-A</t>
-  </si>
-  <si>
-    <t>CS103L-B</t>
-  </si>
-  <si>
-    <t>NS104L-A</t>
-  </si>
-  <si>
-    <t>NS104L-B</t>
-  </si>
-  <si>
-    <t>CS104L-A</t>
-  </si>
-  <si>
-    <t>CS104L-B</t>
-  </si>
-  <si>
-    <t>CS201L</t>
-  </si>
-  <si>
-    <t>CS203L</t>
-  </si>
-  <si>
-    <t>CS204L</t>
-  </si>
-  <si>
-    <t>CS206L</t>
+    <t>CS102A-L1</t>
+  </si>
+  <si>
+    <t>CS102A-L2</t>
+  </si>
+  <si>
+    <t>CS102B-L1</t>
+  </si>
+  <si>
+    <t>CS102B-L2</t>
+  </si>
+  <si>
+    <t>CS101A-L1</t>
+  </si>
+  <si>
+    <t>CS101A-L2</t>
+  </si>
+  <si>
+    <t>CS101B-L</t>
+  </si>
+  <si>
+    <t>CS103A-L</t>
+  </si>
+  <si>
+    <t>CS103B-L</t>
+  </si>
+  <si>
+    <t>NS104A-L</t>
+  </si>
+  <si>
+    <t>NS104B-L</t>
+  </si>
+  <si>
+    <t>CS104A-L</t>
+  </si>
+  <si>
+    <t>CS104B-L</t>
+  </si>
+  <si>
+    <t>CS201-L</t>
+  </si>
+  <si>
+    <t>CS203-L</t>
+  </si>
+  <si>
+    <t>CS204-L</t>
+  </si>
+  <si>
+    <t>CS206-L</t>
   </si>
 </sst>
 </file>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>